<commit_message>
Completed code for project 2
</commit_message>
<xml_diff>
--- a/Proj1Chart.xlsx
+++ b/Proj1Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>NODENUM</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -61,12 +61,15 @@
     <t>Max Speedup</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>1/(1-0.9394391)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,13 +116,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,7 +151,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -167,8 +182,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -294,28 +321,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11.88</c:v>
+                  <c:v>10.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.23</c:v>
+                  <c:v>10.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.78</c:v>
+                  <c:v>10.130000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.89</c:v>
+                  <c:v>10.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.23</c:v>
+                  <c:v>11.92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.39</c:v>
+                  <c:v>11.17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.3</c:v>
+                  <c:v>11.43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.08</c:v>
+                  <c:v>12.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,28 +441,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>24.66</c:v>
+                  <c:v>13.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.89</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.88</c:v>
+                  <c:v>20.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.03</c:v>
+                  <c:v>24.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.79</c:v>
+                  <c:v>24.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.41</c:v>
+                  <c:v>25.21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.11</c:v>
+                  <c:v>24.46</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.39</c:v>
+                  <c:v>25.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,28 +561,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>26.47</c:v>
+                  <c:v>26.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.06</c:v>
+                  <c:v>26.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.32</c:v>
+                  <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.56</c:v>
+                  <c:v>49.86</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.37</c:v>
+                  <c:v>47.64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.37</c:v>
+                  <c:v>49.62</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.08</c:v>
+                  <c:v>47.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49.08</c:v>
+                  <c:v>49.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,28 +681,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>52.79</c:v>
+                  <c:v>39.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.8</c:v>
+                  <c:v>49.31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.64</c:v>
+                  <c:v>51.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.58</c:v>
+                  <c:v>69.09</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.709999999999994</c:v>
+                  <c:v>92.98</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.6</c:v>
+                  <c:v>97.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.98</c:v>
+                  <c:v>98.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.23</c:v>
+                  <c:v>97.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,16 +1087,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.88</c:v>
+                  <c:v>10.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.66</c:v>
+                  <c:v>13.42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.47</c:v>
+                  <c:v>26.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.79</c:v>
+                  <c:v>39.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,16 +1183,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.23</c:v>
+                  <c:v>10.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.89</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.06</c:v>
+                  <c:v>26.83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.8</c:v>
+                  <c:v>49.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,16 +1279,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.78</c:v>
+                  <c:v>10.130000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.88</c:v>
+                  <c:v>20.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.32</c:v>
+                  <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.64</c:v>
+                  <c:v>51.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,16 +1375,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.89</c:v>
+                  <c:v>10.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.03</c:v>
+                  <c:v>24.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.56</c:v>
+                  <c:v>49.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.58</c:v>
+                  <c:v>69.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1444,16 +1471,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.23</c:v>
+                  <c:v>11.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.79</c:v>
+                  <c:v>24.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.37</c:v>
+                  <c:v>47.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.709999999999994</c:v>
+                  <c:v>88.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1540,16 +1567,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.39</c:v>
+                  <c:v>11.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.41</c:v>
+                  <c:v>25.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.37</c:v>
+                  <c:v>49.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.6</c:v>
+                  <c:v>97.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1642,16 +1669,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.3</c:v>
+                  <c:v>11.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.11</c:v>
+                  <c:v>24.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.08</c:v>
+                  <c:v>47.98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.98</c:v>
+                  <c:v>98.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,16 +1771,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.08</c:v>
+                  <c:v>12.27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.39</c:v>
+                  <c:v>25.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.08</c:v>
+                  <c:v>49.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.23</c:v>
+                  <c:v>97.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3425,23 +3452,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04A625B-B884-2849-B81B-C619C279A7D5}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -3468,16 +3497,16 @@
         <v>400</v>
       </c>
       <c r="C3" s="1">
-        <v>11.88</v>
+        <v>10.41</v>
       </c>
       <c r="D3" s="1">
-        <v>24.66</v>
+        <v>13.42</v>
       </c>
       <c r="E3" s="1">
-        <v>26.47</v>
+        <v>26.48</v>
       </c>
       <c r="F3" s="1">
-        <v>52.79</v>
+        <v>39.07</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="s">
@@ -3490,16 +3519,16 @@
         <v>1000</v>
       </c>
       <c r="C4" s="1">
-        <v>11.23</v>
+        <v>10.44</v>
       </c>
       <c r="D4" s="1">
-        <v>24.89</v>
+        <v>13.5</v>
       </c>
       <c r="E4" s="1">
-        <v>31.06</v>
+        <v>26.83</v>
       </c>
       <c r="F4" s="1">
-        <v>62.8</v>
+        <v>49.31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
@@ -3508,16 +3537,16 @@
         <v>2000</v>
       </c>
       <c r="C5" s="1">
-        <v>11.78</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>24.88</v>
+        <v>20.54</v>
       </c>
       <c r="E5" s="1">
-        <v>34.32</v>
+        <v>28.01</v>
       </c>
       <c r="F5" s="1">
-        <v>68.64</v>
+        <v>51.11</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
@@ -3526,16 +3555,16 @@
         <v>4000</v>
       </c>
       <c r="C6" s="1">
-        <v>11.89</v>
+        <v>10.84</v>
       </c>
       <c r="D6" s="1">
-        <v>25.03</v>
+        <v>24.38</v>
       </c>
       <c r="E6" s="1">
-        <v>29.56</v>
+        <v>49.86</v>
       </c>
       <c r="F6" s="1">
-        <v>74.58</v>
+        <v>69.09</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
@@ -3544,16 +3573,16 @@
         <v>6000</v>
       </c>
       <c r="C7" s="1">
-        <v>12.23</v>
+        <v>11.92</v>
       </c>
       <c r="D7" s="1">
-        <v>24.79</v>
+        <v>24.2</v>
       </c>
       <c r="E7" s="1">
-        <v>46.37</v>
+        <v>47.64</v>
       </c>
       <c r="F7" s="1">
-        <v>75.709999999999994</v>
+        <v>92.98</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
@@ -3562,16 +3591,16 @@
         <v>8000</v>
       </c>
       <c r="C8" s="1">
-        <v>12.39</v>
+        <v>11.17</v>
       </c>
       <c r="D8" s="1">
-        <v>24.41</v>
+        <v>25.21</v>
       </c>
       <c r="E8" s="1">
-        <v>46.37</v>
+        <v>49.62</v>
       </c>
       <c r="F8" s="1">
-        <v>88.6</v>
+        <v>97.76</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
@@ -3580,16 +3609,16 @@
         <v>10000</v>
       </c>
       <c r="C9" s="1">
-        <v>12.3</v>
+        <v>11.43</v>
       </c>
       <c r="D9" s="1">
-        <v>24.11</v>
+        <v>24.46</v>
       </c>
       <c r="E9" s="1">
-        <v>49.08</v>
+        <v>47.98</v>
       </c>
       <c r="F9" s="1">
-        <v>86.98</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
@@ -3598,205 +3627,194 @@
         <v>12000</v>
       </c>
       <c r="C10" s="1">
-        <v>12.08</v>
+        <v>12.27</v>
       </c>
       <c r="D10" s="1">
-        <v>24.39</v>
+        <v>25.55</v>
       </c>
       <c r="E10" s="1">
-        <v>49.08</v>
+        <v>49.76</v>
       </c>
       <c r="F10" s="1">
-        <v>86.23</v>
+        <v>97.03</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4">
         <f>D3/C3</f>
-        <v>2.0757575757575757</v>
+        <v>1.2891450528338135</v>
       </c>
       <c r="E12" s="4">
         <f>E3/C3</f>
-        <v>2.2281144781144779</v>
+        <v>2.5437079731027858</v>
       </c>
       <c r="F12" s="4">
         <f>F3/C3</f>
-        <v>4.4436026936026929</v>
+        <v>3.7531219980787704</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="16">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
         <f t="shared" ref="D13:D19" si="0">D4/C4</f>
-        <v>2.2163846838824575</v>
+        <v>1.2931034482758621</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13:E19" si="1">E4/C4</f>
-        <v>2.7658058771148708</v>
+        <v>2.5699233716475094</v>
       </c>
       <c r="F13" s="4">
         <f>F4/C4</f>
-        <v>5.5921638468388242</v>
+        <v>4.7231800766283527</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="16">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
-        <v>2.1120543293718166</v>
+        <v>2.0276406712734452</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>2.913412563667233</v>
+        <v>2.7650542941757155</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" ref="F14:F19" si="2">F5/C5</f>
-        <v>5.826825127334466</v>
+        <v>5.0454096742349455</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="16">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4">
         <f>D6/C6</f>
-        <v>2.105130361648444</v>
+        <v>2.2490774907749076</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>2.486122792262405</v>
+        <v>4.5996309963099629</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
-        <v>6.2724978973927668</v>
+        <v>6.3736162361623618</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="16">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4">
         <f t="shared" si="0"/>
-        <v>2.0269828291087491</v>
+        <v>2.0302013422818792</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>3.791496320523303</v>
+        <v>3.9966442953020134</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
-        <v>6.1905151267375302</v>
+        <v>7.800335570469799</v>
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="16">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:8" ht="16">
+      <c r="A17" s="12"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
-        <v>1.9701372074253429</v>
+        <v>2.2569382273948078</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>3.7425343018563355</v>
+        <v>4.4422560429722466</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>7.1509281678773196</v>
+        <v>8.7520143240823636</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="16">
-      <c r="A18" s="10"/>
+    <row r="18" spans="1:8" ht="16">
+      <c r="A18" s="12"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>1.9601626016260161</v>
+        <v>2.1399825021872267</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>3.9902439024390239</v>
+        <v>4.197725284339457</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>7.0715447154471542</v>
+        <v>8.6351706036745419</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="16">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:8" ht="16">
+      <c r="A19" s="12"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
-        <v>2.0190397350993377</v>
+        <v>2.082314588427058</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>4.0629139072847682</v>
+        <v>4.0554197229013855</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>7.1382450331125833</v>
+        <v>7.9079054604726977</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="16">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:8" ht="16">
+      <c r="A20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5">
         <f>AVERAGE(D12:D19)</f>
-        <v>2.0607061654899672</v>
+        <v>1.921050415431125</v>
       </c>
       <c r="E20" s="5">
         <f>AVERAGE(E12:E19)</f>
-        <v>3.2475805179078021</v>
+        <v>3.6462952475938843</v>
       </c>
       <c r="F20" s="5">
         <f>AVERAGE(F12:F19)</f>
-        <v>6.2107903260429174</v>
+        <v>6.6238442429754789</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="16">
-      <c r="A21" s="4" t="s">
-        <v>8</v>
-      </c>
+    <row r="21" spans="1:8" ht="16">
+      <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="5">
-        <f>MAX(D12:D19)</f>
-        <v>2.2163846838824575</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" ref="E21:F21" si="3">MAX(E12:E19)</f>
-        <v>4.0629139072847682</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="3"/>
-        <v>7.1509281678773196</v>
-      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="16">
+    <row r="22" spans="1:8" ht="16">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3805,193 +3823,209 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="16">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:8" ht="16">
+      <c r="A23" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4">
         <f>(D2/(D2-1))*(1-(1/(D12)))</f>
-        <v>1.0364963503649633</v>
+        <v>0.44858420268256327</v>
       </c>
       <c r="E23" s="4">
         <f>(E2/(E2-1))*(1-(1/(E12)))</f>
-        <v>0.73492003526004268</v>
+        <v>0.80916414904330303</v>
       </c>
       <c r="F23" s="4">
         <f>(F2/(F2-1))*(1-(1/(F12)))</f>
-        <v>0.88566557519010625</v>
+        <v>0.83834875132545983</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="16">
-      <c r="A24" s="9"/>
+    <row r="24" spans="1:8" ht="16">
+      <c r="A24" s="13"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4">
         <f>(D2/(D2-1))*(1-(1/(D13)))</f>
-        <v>1.0976295701084773</v>
+        <v>0.45333333333333337</v>
       </c>
       <c r="E24" s="4">
         <f>(E2/(E2-1))*(1-(1/(E13)))</f>
-        <v>0.85125563425627804</v>
+        <v>0.81451111939371335</v>
       </c>
       <c r="F24" s="4">
         <f>(F2/(F2-1))*(1-(1/(F13)))</f>
-        <v>0.9384895359417651</v>
+        <v>0.9008894168091085</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="16">
-      <c r="A25" s="9"/>
+    <row r="25" spans="1:8" ht="16">
+      <c r="A25" s="13"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4">
         <f>(D2/(D2-1))*(1-(1/(D14)))</f>
-        <v>1.0530546623794212</v>
+        <v>1.0136319376825704</v>
       </c>
       <c r="E25" s="4">
         <f>(E2/(E2-1))*(1-(1/(E14)))</f>
-        <v>0.87567987567987571</v>
+        <v>0.85112459835772936</v>
       </c>
       <c r="F25" s="4">
         <f>(F2/(F2-1))*(1-(1/(F14)))</f>
-        <v>0.94671994671994675</v>
+        <v>0.9163429018643261</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="16">
-      <c r="A26" s="9"/>
+    <row r="26" spans="1:8" ht="16">
+      <c r="A26" s="13"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4">
         <f>(D2/(D2-1))*(1-(1/(D15)))</f>
-        <v>1.0499400719137035</v>
+        <v>1.1107465135356849</v>
       </c>
       <c r="E26" s="4">
         <f>(E2/(E2-1))*(1-(1/(E15)))</f>
-        <v>0.79702300405953985</v>
+        <v>1.0434550073539244</v>
       </c>
       <c r="F26" s="4">
         <f>(F2/(F2-1))*(1-(1/(F15)))</f>
-        <v>0.9606558633107305</v>
+        <v>0.96354651283005599</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="16">
-      <c r="A27" s="9"/>
+    <row r="27" spans="1:8" ht="16">
+      <c r="A27" s="13"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4">
         <f>(D2/(D2-1))*(1-(1/(D16)))</f>
-        <v>1.0133118192819686</v>
+        <v>1.0148760330578512</v>
       </c>
       <c r="E27" s="4">
         <f>(E2/(E2-1))*(1-(1/(E16)))</f>
-        <v>0.98166918266120329</v>
+        <v>0.99972012314581582</v>
       </c>
       <c r="F27" s="4">
         <f>(F2/(F2-1))*(1-(1/(F16)))</f>
-        <v>0.95824291941053263</v>
+        <v>0.99634329963432988</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="16">
-      <c r="A28" s="9"/>
+    <row r="28" spans="1:8" ht="16">
+      <c r="A28" s="13"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4">
         <f>(D2/(D2-1))*(1-(1/(D17)))</f>
-        <v>0.98484227775501831</v>
+        <v>1.1138437128123762</v>
       </c>
       <c r="E28" s="4">
         <f>(E2/(E2-1))*(1-(1/(E17)))</f>
-        <v>0.97706850693695624</v>
+        <v>1.033185543463657</v>
       </c>
       <c r="F28" s="4">
         <f>(F2/(F2-1))*(1-(1/(F17)))</f>
-        <v>0.98303772976459203</v>
+        <v>1.0122749590834696</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="16">
-      <c r="A29" s="9"/>
+    <row r="29" spans="1:8" ht="16">
+      <c r="A29" s="13"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4">
         <f>(D2/(D2-1))*(1-(1/(D18)))</f>
-        <v>0.97967648278722508</v>
+        <v>1.0654129190515127</v>
       </c>
       <c r="E29" s="4">
         <f>(E2/(E2-1))*(1-(1/(E18)))</f>
-        <v>0.99918500407497945</v>
+        <v>1.015700986522162</v>
       </c>
       <c r="F29" s="4">
         <f>(F2/(F2-1))*(1-(1/(F18)))</f>
-        <v>0.98124363564694672</v>
+        <v>1.0105080330004341</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="16">
-      <c r="A30" s="9"/>
+    <row r="30" spans="1:8" ht="16">
+      <c r="A30" s="13"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4">
         <f>(D2/(D2-1))*(1-(1/(D19)))</f>
-        <v>1.0094300943009431</v>
+        <v>1.0395303326810177</v>
       </c>
       <c r="E30" s="4">
         <f>(E2/(E2-1))*(1-(1/(E19)))</f>
-        <v>1.0051616408584623</v>
+        <v>1.0045551982851018</v>
       </c>
       <c r="F30" s="4">
         <f>(F2/(F2-1))*(1-(1/(F19)))</f>
-        <v>0.98275376484816357</v>
+        <v>0.99833630246904492</v>
       </c>
       <c r="G30" s="4"/>
+      <c r="H30" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="31" spans="1:7" ht="16">
-      <c r="A31" s="9"/>
+    <row r="31" spans="1:8" ht="16">
+      <c r="A31" s="13"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4">
         <f>(D2/(D2-1))*(1-(1/(D20)))</f>
-        <v>1.0294589138939823</v>
+        <v>0.95890290856778115</v>
       </c>
       <c r="E31" s="4">
         <f>(E2/(E2-1))*(1-(1/(E20)))</f>
-        <v>0.92277127767957223</v>
+        <v>0.96766537646309003</v>
       </c>
       <c r="F31" s="4">
         <f>(F2/(F2-1))*(1-(1/(F20)))</f>
-        <v>0.95884559475110787</v>
+        <v>0.97032030458997931</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:8" ht="16">
+      <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5">
         <f>AVERAGE(D23:D31)</f>
-        <v>1.0282044714206338</v>
+        <v>0.91320687704496573</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" ref="E32:F32" si="4">AVERAGE(E23:E31)</f>
-        <v>0.90497046238521228</v>
+        <f t="shared" ref="E32:F32" si="3">AVERAGE(E23:E31)</f>
+        <v>0.94878690022538847</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="4"/>
-        <v>0.95507272950932121</v>
+        <f t="shared" si="3"/>
+        <v>0.95632338684513429</v>
       </c>
       <c r="G32" s="6">
         <f>AVERAGE(D32:F32)</f>
-        <v>0.96274922110505579</v>
+        <v>0.93943905470516287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <f>1/(1-G32)</f>
+        <v>16.512291793524081</v>
+      </c>
+      <c r="H33">
+        <f>1-G32</f>
+        <v>6.0560945294837132E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16">
@@ -4042,28 +4076,28 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>11.88</v>
+        <v>10.41</v>
       </c>
       <c r="D37" s="1">
-        <v>11.23</v>
+        <v>10.44</v>
       </c>
       <c r="E37" s="1">
-        <v>11.78</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="F37" s="1">
-        <v>11.89</v>
+        <v>10.84</v>
       </c>
       <c r="G37" s="1">
-        <v>12.23</v>
+        <v>11.92</v>
       </c>
       <c r="H37" s="1">
-        <v>12.39</v>
+        <v>11.17</v>
       </c>
       <c r="I37" s="1">
-        <v>12.3</v>
+        <v>11.43</v>
       </c>
       <c r="J37" s="1">
-        <v>12.08</v>
+        <v>12.27</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4072,28 +4106,28 @@
         <v>2</v>
       </c>
       <c r="C38" s="1">
-        <v>24.66</v>
+        <v>13.42</v>
       </c>
       <c r="D38" s="1">
-        <v>24.89</v>
+        <v>13.5</v>
       </c>
       <c r="E38" s="1">
-        <v>24.88</v>
+        <v>20.54</v>
       </c>
       <c r="F38" s="1">
-        <v>25.03</v>
+        <v>24.38</v>
       </c>
       <c r="G38" s="1">
-        <v>24.79</v>
+        <v>24.2</v>
       </c>
       <c r="H38" s="1">
-        <v>24.41</v>
+        <v>25.21</v>
       </c>
       <c r="I38" s="1">
-        <v>24.11</v>
+        <v>24.46</v>
       </c>
       <c r="J38" s="1">
-        <v>24.39</v>
+        <v>25.55</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4102,28 +4136,28 @@
         <v>4</v>
       </c>
       <c r="C39" s="1">
-        <v>26.47</v>
+        <v>26.48</v>
       </c>
       <c r="D39" s="1">
-        <v>31.06</v>
+        <v>26.83</v>
       </c>
       <c r="E39" s="1">
-        <v>34.32</v>
+        <v>28.01</v>
       </c>
       <c r="F39" s="1">
-        <v>29.56</v>
+        <v>49.86</v>
       </c>
       <c r="G39" s="1">
-        <v>46.37</v>
+        <v>47.64</v>
       </c>
       <c r="H39" s="1">
-        <v>46.37</v>
+        <v>49.62</v>
       </c>
       <c r="I39" s="1">
-        <v>49.08</v>
+        <v>47.98</v>
       </c>
       <c r="J39" s="1">
-        <v>49.08</v>
+        <v>49.76</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4132,28 +4166,28 @@
         <v>8</v>
       </c>
       <c r="C40" s="1">
-        <v>52.79</v>
+        <v>39.07</v>
       </c>
       <c r="D40" s="1">
-        <v>62.8</v>
+        <v>49.31</v>
       </c>
       <c r="E40" s="1">
-        <v>68.64</v>
+        <v>51.11</v>
       </c>
       <c r="F40" s="1">
-        <v>74.58</v>
+        <v>69.09</v>
       </c>
       <c r="G40" s="1">
-        <v>75.709999999999994</v>
+        <v>88.98</v>
       </c>
       <c r="H40" s="1">
-        <v>88.6</v>
+        <v>97.76</v>
       </c>
       <c r="I40" s="1">
-        <v>86.98</v>
+        <v>98.7</v>
       </c>
       <c r="J40" s="1">
-        <v>86.23</v>
+        <v>97.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>